<commit_message>
update schematic & BOM
</commit_message>
<xml_diff>
--- a/03_BOM/LASER_EXT_BOM.xlsx
+++ b/03_BOM/LASER_EXT_BOM.xlsx
@@ -5,18 +5,18 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\LAB\LASER\03_BOM\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\NANORACK_V2_LASER_EXT_HW\03_BOM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7ECCF5A7-20EF-4951-BF70-B2F1E46C2EAC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B4FAE9C-6E6B-4944-A947-05404C0C35A9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{8FC6FF28-B623-4847-BFCE-4450D015DC43}"/>
+    <workbookView xWindow="19090" yWindow="-1950" windowWidth="25820" windowHeight="15500" xr2:uid="{83B2A217-D66D-4505-985B-7E3BE10BA6E9}"/>
   </bookViews>
   <sheets>
-    <sheet name="NANORACK_EXT_LASER" sheetId="1" r:id="rId1"/>
+    <sheet name="LASER_EXT_BOM" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Titles" localSheetId="0">NANORACK_EXT_LASER!$1:$1</definedName>
+    <definedName name="_xlnm.Print_Titles" localSheetId="0">LASER_EXT_BOM!$1:$1</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -81,7 +81,7 @@
     <t>RES SMD 22 OHM 1% 1/10W 0603</t>
   </si>
   <si>
-    <t>R2, R3, R4, R6</t>
+    <t>R3, R4, R5, R6</t>
   </si>
   <si>
     <t>RES-SMD-0603</t>
@@ -99,7 +99,7 @@
     <t>RES SMD 4.7K OHM 1% 1/10W 0603</t>
   </si>
   <si>
-    <t>R1, R5</t>
+    <t>R1, R2</t>
   </si>
   <si>
     <t>ERJ-3EKF4701V</t>
@@ -186,7 +186,7 @@
     <t>TESTPOINT</t>
   </si>
   <si>
-    <t>SOD123</t>
+    <t>SOD-123</t>
   </si>
 </sst>
 </file>
@@ -562,11 +562,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E524A345-28C0-4186-80BA-EA6827EAA7A9}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E3D4AD37-0CF5-4C92-8ACA-2A1205943BF5}">
   <dimension ref="A1:G11"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -574,7 +574,7 @@
     <col min="1" max="1" width="17.140625" customWidth="1"/>
     <col min="2" max="2" width="36" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="34" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.7109375" customWidth="1"/>
     <col min="5" max="5" width="24.5703125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="27.5703125" customWidth="1"/>
     <col min="7" max="7" width="11.28515625" customWidth="1"/>

</xml_diff>